<commit_message>
requirement to release QMS
captured, analyzed and mentioned repository versions.
</commit_message>
<xml_diff>
--- a/PEG_QMSREQ.xlsx
+++ b/PEG_QMSREQ.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7260" tabRatio="879" firstSheet="8" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7260" tabRatio="879" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="QMS_Next Change Requirement (2" sheetId="12" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="QMS_3.0 Change Requirements" sheetId="13" r:id="rId10"/>
     <sheet name="QMS_3.1 Change Requirements" sheetId="14" r:id="rId11"/>
     <sheet name="QMS_4.0 Change Requirements" sheetId="15" r:id="rId12"/>
+    <sheet name="QMS_4.1 Change Requirements" sheetId="16" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="324">
   <si>
     <t>Genus Innovation Limited</t>
   </si>
@@ -1036,6 +1037,105 @@
   </si>
   <si>
     <t>Training Module of Einframe</t>
+  </si>
+  <si>
+    <t>For new segment  project  effort estimation template need to more align .</t>
+  </si>
+  <si>
+    <t>Designer itself do module testing by making module test cases, so to do this formally like log the defects and resolve by himself is extra burden, practically it is part of design &amp; implementation and do in each projects. So see this and revise processes accordingly.</t>
+  </si>
+  <si>
+    <t>Audit repitition in a phase : before and after Metrics report audit is time consuming for team, pls change to to once after metrics report preparation only.</t>
+  </si>
+  <si>
+    <t>Audit checklist to be sync with GIL.ef : Category of NC is to be sync with term functional/non-functional</t>
+  </si>
+  <si>
+    <t>Audit Chaecklist updation w.r.t. Einframe</t>
+  </si>
+  <si>
+    <t>External Review (IR)</t>
+  </si>
+  <si>
+    <t>Measurement Goals should have some relastic figures, should not zero</t>
+  </si>
+  <si>
+    <t>Size via complexity should reflect in efforts estimation template</t>
+  </si>
+  <si>
+    <t>Audit checklist</t>
+  </si>
+  <si>
+    <t>Efforts Estimation Template</t>
+  </si>
+  <si>
+    <t>Project Plan Procedure</t>
+  </si>
+  <si>
+    <t>Implementation Procedure, Module Test Cases</t>
+  </si>
+  <si>
+    <t>Google form for Training feedback need to mention</t>
+  </si>
+  <si>
+    <t>By Training coordinator</t>
+  </si>
+  <si>
+    <t>OT procedure</t>
+  </si>
+  <si>
+    <t>Repository Rev.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">size in terms of Complexity more clearly defined and to identify complexity guidelines added. </t>
+  </si>
+  <si>
+    <t>Updated in planning procedure</t>
+  </si>
+  <si>
+    <t>Major and Minor words replaced by Functional &amp; Non-Functional respectively</t>
+  </si>
+  <si>
+    <t>Organization performance goal page of Einframe</t>
+  </si>
+  <si>
+    <t>Line rejection ration goal changed to 2.5</t>
+  </si>
+  <si>
+    <t>Training feedback google form link mentioned in Training procedure.</t>
+  </si>
+  <si>
+    <t>Already mentioned that log the incidents if required</t>
+  </si>
+  <si>
+    <t>2e7743a70c945aebc315fb7c8b0b270613d02a22</t>
+  </si>
+  <si>
+    <t>547dbdc3cd09e7b9ecad634eef0fc5691115e6ea</t>
+  </si>
+  <si>
+    <t>be4787ad0e20208cfa1468e98429759a70c40490</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Asset, knowledge, technology related points mentioned in checklist</t>
+  </si>
+  <si>
+    <t>13ef27ab8de43dec6dd69d89d39a7c1414861a46</t>
+  </si>
+  <si>
+    <t>96f68c42cf66a5a78399585f9ae1844f99a0d590</t>
+  </si>
+  <si>
+    <t>Estimation : Size in terms of complexity</t>
+  </si>
+  <si>
+    <t>Escalation Guidelines</t>
+  </si>
+  <si>
+    <t>Training feedback google form</t>
   </si>
 </sst>
 </file>
@@ -1138,7 +1238,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
@@ -1181,13 +1281,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1197,7 +1300,100 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="114">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor rgb="FF000000"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2022,25 +2218,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1463578" displayName="Table1463578" ref="A5:H19" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table1463578" displayName="Table1463578" ref="A5:H19" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="A5:H19"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="100"/>
-    <tableColumn id="2" name="Input" dataDxfId="99"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="98"/>
-    <tableColumn id="4" name="Decision" dataDxfId="97"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="96"/>
-    <tableColumn id="8" name="Size" dataDxfId="95"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="94"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="93"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="111"/>
+    <tableColumn id="2" name="Input" dataDxfId="110"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="109"/>
+    <tableColumn id="4" name="Decision" dataDxfId="108"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="107"/>
+    <tableColumn id="8" name="Size" dataDxfId="106"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="105"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14635791011" displayName="Table14635791011" ref="A5:I27" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table14635791011" displayName="Table14635791011" ref="A5:I27" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A5:I27"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Sr. No." dataDxfId="19"/>
+    <tableColumn id="2" name="Input" dataDxfId="18"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="17"/>
+    <tableColumn id="4" name="Decision" dataDxfId="16"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="15"/>
+    <tableColumn id="8" name="Size" dataDxfId="14"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="13"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="12"/>
+    <tableColumn id="9" name="Impact on Projects" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1463579101112" displayName="Table1463579101112" ref="A5:I26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A5:I26"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Sr. No." dataDxfId="8"/>
     <tableColumn id="2" name="Input" dataDxfId="7"/>
@@ -2049,7 +2263,7 @@
     <tableColumn id="7" name="Artefacts to be modified" dataDxfId="4"/>
     <tableColumn id="8" name="Size" dataDxfId="3"/>
     <tableColumn id="5" name="Remarks" dataDxfId="2"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="1"/>
+    <tableColumn id="6" name="Repository Rev." dataDxfId="1"/>
     <tableColumn id="9" name="Impact on Projects" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2057,109 +2271,127 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:H30" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A5:H30" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A5:H30"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="90"/>
-    <tableColumn id="2" name="Input" dataDxfId="89"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="88"/>
-    <tableColumn id="4" name="Decision" dataDxfId="87"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="86"/>
-    <tableColumn id="8" name="Size" dataDxfId="85"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="84"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="83"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="101"/>
+    <tableColumn id="2" name="Input" dataDxfId="100"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="99"/>
+    <tableColumn id="4" name="Decision" dataDxfId="98"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="97"/>
+    <tableColumn id="8" name="Size" dataDxfId="96"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="95"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A5:H26" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A5:H26" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <autoFilter ref="A5:H26"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="80"/>
-    <tableColumn id="2" name="Input" dataDxfId="79"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="78"/>
-    <tableColumn id="4" name="Decision" dataDxfId="77"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="76"/>
-    <tableColumn id="8" name="Size" dataDxfId="75"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="74"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="73"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="91"/>
+    <tableColumn id="2" name="Input" dataDxfId="90"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="89"/>
+    <tableColumn id="4" name="Decision" dataDxfId="88"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="87"/>
+    <tableColumn id="8" name="Size" dataDxfId="86"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="85"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A5:H12" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table146" displayName="Table146" ref="A5:H12" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A5:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="70"/>
-    <tableColumn id="2" name="Input" dataDxfId="69"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="68"/>
-    <tableColumn id="4" name="Decision" dataDxfId="67"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="66"/>
-    <tableColumn id="8" name="Size" dataDxfId="65"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="64"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="63"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="81"/>
+    <tableColumn id="2" name="Input" dataDxfId="80"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="79"/>
+    <tableColumn id="4" name="Decision" dataDxfId="78"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="77"/>
+    <tableColumn id="8" name="Size" dataDxfId="76"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="75"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1463" displayName="Table1463" ref="A5:H30" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1463" displayName="Table1463" ref="A5:H30" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="A5:H30"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="60"/>
-    <tableColumn id="2" name="Input" dataDxfId="59"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="58"/>
-    <tableColumn id="4" name="Decision" dataDxfId="57"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="56"/>
-    <tableColumn id="8" name="Size" dataDxfId="55"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="54"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="53"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="71"/>
+    <tableColumn id="2" name="Input" dataDxfId="70"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="69"/>
+    <tableColumn id="4" name="Decision" dataDxfId="68"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="67"/>
+    <tableColumn id="8" name="Size" dataDxfId="66"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="65"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table14635" displayName="Table14635" ref="A5:H12" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table14635" displayName="Table14635" ref="A5:H12" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A5:H12"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="50"/>
-    <tableColumn id="2" name="Input" dataDxfId="49"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="48"/>
-    <tableColumn id="4" name="Decision" dataDxfId="47"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="46"/>
-    <tableColumn id="8" name="Size" dataDxfId="45"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="44"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="43"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="61"/>
+    <tableColumn id="2" name="Input" dataDxfId="60"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="59"/>
+    <tableColumn id="4" name="Decision" dataDxfId="58"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="57"/>
+    <tableColumn id="8" name="Size" dataDxfId="56"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="55"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table146357" displayName="Table146357" ref="A5:H24" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table146357" displayName="Table146357" ref="A5:H24" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
   <autoFilter ref="A5:H24"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Sr. No." dataDxfId="40"/>
-    <tableColumn id="2" name="Input" dataDxfId="39"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="38"/>
-    <tableColumn id="4" name="Decision" dataDxfId="37"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="36"/>
-    <tableColumn id="8" name="Size" dataDxfId="35"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="34"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="33"/>
+    <tableColumn id="1" name="Sr. No." dataDxfId="51"/>
+    <tableColumn id="2" name="Input" dataDxfId="50"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="49"/>
+    <tableColumn id="4" name="Decision" dataDxfId="48"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="47"/>
+    <tableColumn id="8" name="Size" dataDxfId="46"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="45"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1463579" displayName="Table1463579" ref="A5:I27" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1463579" displayName="Table1463579" ref="A5:I27" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A5:I27"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Sr. No." dataDxfId="41"/>
+    <tableColumn id="2" name="Input" dataDxfId="40"/>
+    <tableColumn id="3" name="Source of Input" dataDxfId="39"/>
+    <tableColumn id="4" name="Decision" dataDxfId="38"/>
+    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="37"/>
+    <tableColumn id="8" name="Size" dataDxfId="36"/>
+    <tableColumn id="5" name="Remarks" dataDxfId="35"/>
+    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="34"/>
+    <tableColumn id="9" name="Impact on Projects" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table146357910" displayName="Table146357910" ref="A5:I27" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A5:I27"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Sr. No." dataDxfId="30"/>
@@ -2171,24 +2403,6 @@
     <tableColumn id="5" name="Remarks" dataDxfId="24"/>
     <tableColumn id="6" name="SVN Repository Rev." dataDxfId="23"/>
     <tableColumn id="9" name="Impact on Projects" dataDxfId="22"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table146357910" displayName="Table146357910" ref="A5:I27" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
-  <autoFilter ref="A5:I27"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Sr. No." dataDxfId="19"/>
-    <tableColumn id="2" name="Input" dataDxfId="18"/>
-    <tableColumn id="3" name="Source of Input" dataDxfId="17"/>
-    <tableColumn id="4" name="Decision" dataDxfId="16"/>
-    <tableColumn id="7" name="Artefacts to be modified" dataDxfId="15"/>
-    <tableColumn id="8" name="Size" dataDxfId="14"/>
-    <tableColumn id="5" name="Remarks" dataDxfId="13"/>
-    <tableColumn id="6" name="SVN Repository Rev." dataDxfId="12"/>
-    <tableColumn id="9" name="Impact on Projects" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2847,10 +3061,10 @@
       <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -3523,10 +3737,10 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -4013,10 +4227,10 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -4049,7 +4263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -4106,25 +4320,25 @@
       <c r="A6" s="14">
         <v>1</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>283</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>284</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="16" t="s">
         <v>285</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>105</v>
       </c>
       <c r="I6" s="10" t="s">
@@ -4469,10 +4683,10 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="18"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
@@ -4517,6 +4731,574 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A28:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="59.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>316</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>5</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="14">
+        <v>6</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>7</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>9</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>10</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>11</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="14">
+        <v>8</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>20</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="H24" s="14"/>
+      <c r="I24" s="10"/>
+    </row>
+    <row r="25" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>21</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="H25" s="14"/>
+      <c r="I25" s="10"/>
+    </row>
+    <row r="26" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>22</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="10"/>
+    </row>
+    <row r="27" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="13">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5738,10 +6520,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="16"/>
+      <c r="B29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
@@ -6043,10 +6825,10 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -6686,10 +7468,10 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="16"/>
+      <c r="B34" s="17"/>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -6961,10 +7743,10 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="17"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -7522,10 +8304,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="17"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">

</xml_diff>